<commit_message>
indv water quality graphs plus summary stats
</commit_message>
<xml_diff>
--- a/water_quality/samples.xlsx
+++ b/water_quality/samples.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gizmo/Github/emc/water_quality/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D141BC37-35BB-234B-B1DA-3A57D8E90C1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE405512-4B50-DE4C-A7C7-0281EF1A31CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2680" yWindow="900" windowWidth="15820" windowHeight="17040" xr2:uid="{F83C51FD-ACD1-4143-913C-8F92A0F6EC2B}"/>
+    <workbookView xWindow="11600" yWindow="720" windowWidth="15820" windowHeight="17040" xr2:uid="{F83C51FD-ACD1-4143-913C-8F92A0F6EC2B}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_data" sheetId="1" r:id="rId1"/>
@@ -34,65 +34,38 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
   <si>
     <t>Date and time</t>
   </si>
   <si>
-    <t>WQ1</t>
-  </si>
-  <si>
     <t>2021-04-06T13:47:02Z</t>
   </si>
   <si>
-    <t>WQ2</t>
-  </si>
-  <si>
     <t>2021-04-06T14:14:21Z</t>
   </si>
   <si>
-    <t>WQ3</t>
-  </si>
-  <si>
     <t>2021-04-06T14:21:01Z</t>
   </si>
   <si>
-    <t>WQ4</t>
-  </si>
-  <si>
     <t>2021-04-06T14:31:28Z</t>
   </si>
   <si>
-    <t>WQ5</t>
-  </si>
-  <si>
     <t>2021-04-06T14:46:08Z</t>
   </si>
   <si>
-    <t>WQ6</t>
-  </si>
-  <si>
     <t>2021-04-06T14:56:11Z</t>
   </si>
   <si>
-    <t>WQ7</t>
-  </si>
-  <si>
     <t>2021-04-06T15:01:52Z</t>
   </si>
   <si>
     <t>2021-04-06T15:19:12Z</t>
   </si>
   <si>
-    <t>WQ9</t>
-  </si>
-  <si>
     <t>2021-04-06T15:32:41Z</t>
   </si>
   <si>
-    <t>WQ10</t>
-  </si>
-  <si>
     <t>2021-04-06T15:39:14Z</t>
   </si>
   <si>
@@ -105,21 +78,6 @@
     <t>Ten Pound Bay</t>
   </si>
   <si>
-    <t>Great Deep</t>
-  </si>
-  <si>
-    <t>Friar's Head</t>
-  </si>
-  <si>
-    <t>Open water comparison</t>
-  </si>
-  <si>
-    <t>GI Anchorage</t>
-  </si>
-  <si>
-    <t>Dansby Beach</t>
-  </si>
-  <si>
     <t>Club House</t>
   </si>
   <si>
@@ -159,9 +117,6 @@
     <t>Nitrate_raw</t>
   </si>
   <si>
-    <t>WQ8</t>
-  </si>
-  <si>
     <t>ph</t>
   </si>
   <si>
@@ -174,13 +129,61 @@
     <t>Site</t>
   </si>
   <si>
-    <t>sample</t>
-  </si>
-  <si>
-    <t>control</t>
-  </si>
-  <si>
-    <t>Nonsuch</t>
+    <t>treatment</t>
+  </si>
+  <si>
+    <t>Open Water</t>
+  </si>
+  <si>
+    <t>Dansby's Beach</t>
+  </si>
+  <si>
+    <t>exploratory</t>
+  </si>
+  <si>
+    <t>nursery</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>Nonsuch Anchorage</t>
+  </si>
+  <si>
+    <t>T6</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>Big Deep</t>
+  </si>
+  <si>
+    <t>N1</t>
+  </si>
+  <si>
+    <t>N2</t>
+  </si>
+  <si>
+    <t>Friar's Head Bay</t>
+  </si>
+  <si>
+    <t>Green Isl. Anchorage</t>
   </si>
 </sst>
 </file>
@@ -543,73 +546,73 @@
   <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="F2" s="1">
         <v>7.9</v>
@@ -644,19 +647,19 @@
     </row>
     <row r="3" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>47</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="F3" s="1">
         <v>8.11</v>
@@ -691,19 +694,19 @@
     </row>
     <row r="4" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="F4" s="1">
         <v>8.16</v>
@@ -738,19 +741,19 @@
     </row>
     <row r="5" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="F5" s="1">
         <v>8.1880000000000006</v>
@@ -785,19 +788,19 @@
     </row>
     <row r="6" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="F6" s="1">
         <v>8.1300000000000008</v>
@@ -818,7 +821,7 @@
         <v>6.47</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="M6" s="1">
         <v>0.01</v>
@@ -832,19 +835,19 @@
     </row>
     <row r="7" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="F7" s="1">
         <v>8.19</v>
@@ -865,7 +868,7 @@
         <v>7.19</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="M7" s="1">
         <v>0.01</v>
@@ -879,19 +882,19 @@
     </row>
     <row r="8" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="F8" s="1">
         <v>8.2100000000000009</v>
@@ -926,19 +929,19 @@
     </row>
     <row r="9" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="F9" s="1">
         <v>8.18</v>
@@ -973,19 +976,19 @@
     </row>
     <row r="10" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="F10" s="1">
         <v>8.19</v>
@@ -1006,7 +1009,7 @@
         <v>6.47</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="M10" s="1">
         <v>0.01</v>
@@ -1020,19 +1023,19 @@
     </row>
     <row r="11" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="F11" s="1">
         <v>8.19</v>

</xml_diff>

<commit_message>
refining egret result graphs
</commit_message>
<xml_diff>
--- a/water_quality/samples.xlsx
+++ b/water_quality/samples.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gizmo/Github/emc/water_quality/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F0DDFE-A3CE-B04C-A3CF-42555E669761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F8E2C2-911A-3A4A-8FD9-B03E87D21398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9300" yWindow="460" windowWidth="26260" windowHeight="17040" xr2:uid="{F83C51FD-ACD1-4143-913C-8F92A0F6EC2B}"/>
+    <workbookView xWindow="13580" yWindow="460" windowWidth="26260" windowHeight="17040" xr2:uid="{F83C51FD-ACD1-4143-913C-8F92A0F6EC2B}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="59">
   <si>
     <t>Hell's Gate</t>
   </si>
@@ -188,6 +188,30 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>Willoughby</t>
+  </si>
+  <si>
+    <t>Fort Williams</t>
+  </si>
+  <si>
+    <t>Big Deep - mat center</t>
+  </si>
+  <si>
+    <t>Big Deep - mat edge</t>
+  </si>
+  <si>
+    <t>Big Deep - 300m</t>
+  </si>
+  <si>
+    <t>Friar's - mat center</t>
+  </si>
+  <si>
+    <t>Friar's - mat edge</t>
+  </si>
+  <si>
+    <t>Friar's - 300m</t>
   </si>
 </sst>
 </file>
@@ -564,1300 +588,1199 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCE1CC20-21DC-EB48-A8F9-D49E40D1816F}">
-  <dimension ref="A1:P27"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B1" sqref="B1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="3" width="0" hidden="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>23</v>
+      <c r="B2" s="5">
+        <v>44292</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="5">
-        <v>44292</v>
-      </c>
-      <c r="E2" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="D2" s="4">
+        <v>7.9</v>
+      </c>
+      <c r="E2" s="4">
+        <v>35698</v>
+      </c>
       <c r="F2" s="4">
-        <v>7.9</v>
+        <v>54918</v>
       </c>
       <c r="G2" s="4">
-        <v>35698</v>
+        <v>36360</v>
       </c>
       <c r="H2" s="4">
-        <v>54918</v>
+        <v>0.48</v>
       </c>
       <c r="I2" s="4">
-        <v>36360</v>
+        <v>6.48</v>
       </c>
       <c r="J2" s="4">
-        <v>0.48</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="K2" s="4">
-        <v>6.48</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="L2" s="4">
-        <v>7.0000000000000007E-2</v>
+        <v>0.44</v>
       </c>
       <c r="M2" s="4">
-        <v>7.0000000000000007E-2</v>
+        <v>0.44</v>
       </c>
       <c r="N2" s="4">
-        <v>0.44</v>
-      </c>
-      <c r="O2" s="4">
-        <v>0.44</v>
-      </c>
-      <c r="P2" s="4">
         <v>26.3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>24</v>
+      <c r="B3" s="5">
+        <v>44292</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="5">
-        <v>44292</v>
-      </c>
-      <c r="E3" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="D3" s="4">
+        <v>8.11</v>
+      </c>
+      <c r="E3" s="4">
+        <v>35695</v>
+      </c>
       <c r="F3" s="4">
-        <v>8.11</v>
+        <v>54915</v>
       </c>
       <c r="G3" s="4">
-        <v>35695</v>
+        <v>36340</v>
       </c>
       <c r="H3" s="4">
-        <v>54915</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="I3" s="4">
-        <v>36340</v>
+        <v>6.43</v>
       </c>
       <c r="J3" s="4">
-        <v>0.28000000000000003</v>
+        <v>0.03</v>
       </c>
       <c r="K3" s="4">
-        <v>6.43</v>
+        <v>0.03</v>
       </c>
       <c r="L3" s="4">
-        <v>0.03</v>
+        <v>0.15</v>
       </c>
       <c r="M3" s="4">
-        <v>0.03</v>
+        <v>0.15</v>
       </c>
       <c r="N3" s="4">
-        <v>0.15</v>
-      </c>
-      <c r="O3" s="4">
-        <v>0.15</v>
-      </c>
-      <c r="P3" s="4">
         <v>26.3</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>24</v>
+      <c r="B4" s="5">
+        <v>44292</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="5">
-        <v>44292</v>
-      </c>
-      <c r="E4" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="D4" s="4">
+        <v>8.16</v>
+      </c>
+      <c r="E4" s="4">
+        <v>35703</v>
+      </c>
       <c r="F4" s="4">
-        <v>8.16</v>
+        <v>54928</v>
       </c>
       <c r="G4" s="4">
-        <v>35703</v>
+        <v>36350</v>
       </c>
       <c r="H4" s="4">
-        <v>54928</v>
+        <v>0.22</v>
       </c>
       <c r="I4" s="4">
-        <v>36350</v>
+        <v>6.54</v>
       </c>
       <c r="J4" s="4">
-        <v>0.22</v>
+        <v>0.02</v>
       </c>
       <c r="K4" s="4">
-        <v>6.54</v>
+        <v>0.02</v>
       </c>
       <c r="L4" s="4">
-        <v>0.02</v>
+        <v>0.4</v>
       </c>
       <c r="M4" s="4">
-        <v>0.02</v>
+        <v>0.4</v>
       </c>
       <c r="N4" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="O4" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="P4" s="4">
         <v>26.3</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>20</v>
+      <c r="B5" s="5">
+        <v>44292</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="5">
-        <v>44292</v>
-      </c>
-      <c r="E5" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="D5" s="4">
+        <v>8.1880000000000006</v>
+      </c>
+      <c r="E5" s="4">
+        <v>35775</v>
+      </c>
       <c r="F5" s="4">
-        <v>8.1880000000000006</v>
+        <v>55038</v>
       </c>
       <c r="G5" s="4">
-        <v>35775</v>
+        <v>36430</v>
       </c>
       <c r="H5" s="4">
-        <v>55038</v>
+        <v>0.35</v>
       </c>
       <c r="I5" s="4">
-        <v>36430</v>
+        <v>6.26</v>
       </c>
       <c r="J5" s="4">
-        <v>0.35</v>
+        <v>0.08</v>
       </c>
       <c r="K5" s="4">
-        <v>6.26</v>
+        <v>0.08</v>
       </c>
       <c r="L5" s="4">
-        <v>0.08</v>
+        <v>0.47</v>
       </c>
       <c r="M5" s="4">
-        <v>0.08</v>
+        <v>0.47</v>
       </c>
       <c r="N5" s="4">
-        <v>0.47</v>
-      </c>
-      <c r="O5" s="4">
-        <v>0.47</v>
-      </c>
-      <c r="P5" s="4">
         <v>26.5</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>20</v>
+      <c r="B6" s="5">
+        <v>44292</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="5">
-        <v>44292</v>
-      </c>
-      <c r="E6" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="D6" s="4">
+        <v>8.1300000000000008</v>
+      </c>
+      <c r="E6" s="4">
+        <v>35667</v>
+      </c>
       <c r="F6" s="4">
-        <v>8.1300000000000008</v>
+        <v>54872</v>
       </c>
       <c r="G6" s="4">
-        <v>35667</v>
+        <v>36310</v>
       </c>
       <c r="H6" s="4">
-        <v>54872</v>
+        <v>0.39</v>
       </c>
       <c r="I6" s="4">
-        <v>36310</v>
-      </c>
-      <c r="J6" s="4">
-        <v>0.39</v>
+        <v>6.47</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="K6" s="4">
-        <v>6.47</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>14</v>
+        <v>0.01</v>
+      </c>
+      <c r="L6" s="4">
+        <v>0.4</v>
       </c>
       <c r="M6" s="4">
-        <v>0.01</v>
+        <v>0.4</v>
       </c>
       <c r="N6" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="O6" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="P6" s="4">
         <v>26.4</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>20</v>
+      <c r="B7" s="5">
+        <v>44292</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="5">
-        <v>44292</v>
-      </c>
-      <c r="E7" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="D7" s="4">
+        <v>8.19</v>
+      </c>
+      <c r="E7" s="4">
+        <v>35687</v>
+      </c>
       <c r="F7" s="4">
-        <v>8.19</v>
+        <v>54903</v>
       </c>
       <c r="G7" s="4">
-        <v>35687</v>
+        <v>36330</v>
       </c>
       <c r="H7" s="4">
-        <v>54903</v>
+        <v>0.31</v>
       </c>
       <c r="I7" s="4">
-        <v>36330</v>
-      </c>
-      <c r="J7" s="4">
-        <v>0.31</v>
+        <v>7.19</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="K7" s="4">
-        <v>7.19</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>14</v>
+        <v>0.01</v>
+      </c>
+      <c r="L7" s="4">
+        <v>0.4</v>
       </c>
       <c r="M7" s="4">
-        <v>0.01</v>
+        <v>0.4</v>
       </c>
       <c r="N7" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="O7" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="P7" s="4">
         <v>26.4</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>20</v>
+      <c r="B8" s="5">
+        <v>44292</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="5">
-        <v>44292</v>
-      </c>
-      <c r="E8" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="D8" s="4">
+        <v>8.2100000000000009</v>
+      </c>
+      <c r="E8" s="4">
+        <v>35751</v>
+      </c>
       <c r="F8" s="4">
-        <v>8.2100000000000009</v>
+        <v>55002</v>
       </c>
       <c r="G8" s="4">
-        <v>35751</v>
+        <v>36400</v>
       </c>
       <c r="H8" s="4">
-        <v>55002</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="I8" s="4">
-        <v>36400</v>
+        <v>6.96</v>
       </c>
       <c r="J8" s="4">
-        <v>0.28999999999999998</v>
+        <v>0.04</v>
       </c>
       <c r="K8" s="4">
-        <v>6.96</v>
+        <v>0.04</v>
       </c>
       <c r="L8" s="4">
-        <v>0.04</v>
+        <v>0.13</v>
       </c>
       <c r="M8" s="4">
-        <v>0.04</v>
+        <v>0.13</v>
       </c>
       <c r="N8" s="4">
-        <v>0.13</v>
-      </c>
-      <c r="O8" s="4">
-        <v>0.13</v>
-      </c>
-      <c r="P8" s="4">
         <v>26.7</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>23</v>
+      <c r="B9" s="5">
+        <v>44292</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="5">
-        <v>44292</v>
-      </c>
-      <c r="E9" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="D9" s="4">
+        <v>8.18</v>
+      </c>
+      <c r="E9" s="4">
+        <v>35705</v>
+      </c>
       <c r="F9" s="4">
-        <v>8.18</v>
+        <v>54930</v>
       </c>
       <c r="G9" s="4">
-        <v>35705</v>
+        <v>36360</v>
       </c>
       <c r="H9" s="4">
-        <v>54930</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="I9" s="4">
-        <v>36360</v>
+        <v>6.51</v>
       </c>
       <c r="J9" s="4">
-        <v>0.28000000000000003</v>
+        <v>0.08</v>
       </c>
       <c r="K9" s="4">
-        <v>6.51</v>
+        <v>0.08</v>
       </c>
       <c r="L9" s="4">
-        <v>0.08</v>
+        <v>0.37</v>
       </c>
       <c r="M9" s="4">
-        <v>0.08</v>
+        <v>0.37</v>
       </c>
       <c r="N9" s="4">
-        <v>0.37</v>
-      </c>
-      <c r="O9" s="4">
-        <v>0.37</v>
-      </c>
-      <c r="P9" s="4">
         <v>26.2</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>20</v>
+      <c r="B10" s="5">
+        <v>44292</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="5">
-        <v>44292</v>
-      </c>
-      <c r="E10" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="D10" s="4">
+        <v>8.19</v>
+      </c>
+      <c r="E10" s="4">
+        <v>35738</v>
+      </c>
       <c r="F10" s="4">
-        <v>8.19</v>
+        <v>54982</v>
       </c>
       <c r="G10" s="4">
-        <v>35738</v>
+        <v>36390</v>
       </c>
       <c r="H10" s="4">
-        <v>54982</v>
+        <v>0.38</v>
       </c>
       <c r="I10" s="4">
-        <v>36390</v>
-      </c>
-      <c r="J10" s="4">
-        <v>0.38</v>
+        <v>6.47</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="K10" s="4">
-        <v>6.47</v>
-      </c>
-      <c r="L10" s="4" t="s">
-        <v>14</v>
+        <v>0.01</v>
+      </c>
+      <c r="L10" s="4">
+        <v>0.28000000000000003</v>
       </c>
       <c r="M10" s="4">
-        <v>0.01</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="N10" s="4">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="O10" s="4">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="P10" s="4">
         <v>26.3</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>20</v>
+      <c r="B11" s="5">
+        <v>44292</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="5">
-        <v>44292</v>
-      </c>
-      <c r="E11" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="D11" s="4">
+        <v>8.19</v>
+      </c>
+      <c r="E11" s="4">
+        <v>35801</v>
+      </c>
       <c r="F11" s="4">
-        <v>8.19</v>
+        <v>55079</v>
       </c>
       <c r="G11" s="4">
-        <v>35801</v>
+        <v>36460</v>
       </c>
       <c r="H11" s="4">
-        <v>55079</v>
+        <v>0.33</v>
       </c>
       <c r="I11" s="4">
-        <v>36460</v>
+        <v>6.63</v>
       </c>
       <c r="J11" s="4">
-        <v>0.33</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="K11" s="4">
-        <v>6.63</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="L11" s="4">
-        <v>7.0000000000000007E-2</v>
+        <v>0.41</v>
       </c>
       <c r="M11" s="4">
-        <v>7.0000000000000007E-2</v>
+        <v>0.41</v>
       </c>
       <c r="N11" s="4">
-        <v>0.41</v>
-      </c>
-      <c r="O11" s="4">
-        <v>0.41</v>
-      </c>
-      <c r="P11" s="4">
         <v>26.5</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5">
+      <c r="B12" s="5">
         <v>44419</v>
       </c>
+      <c r="C12" s="2">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2">
+        <v>7.91</v>
+      </c>
       <c r="E12" s="2">
-        <v>2</v>
+        <v>36660</v>
       </c>
       <c r="F12" s="2">
-        <v>7.91</v>
+        <v>55720</v>
       </c>
       <c r="G12" s="2">
-        <v>36660</v>
+        <v>31850</v>
       </c>
       <c r="H12" s="2">
-        <v>55720</v>
+        <v>1.58</v>
       </c>
       <c r="I12" s="2">
-        <v>31850</v>
-      </c>
-      <c r="J12" s="2">
-        <v>1.58</v>
-      </c>
-      <c r="K12" s="2">
         <v>6.84</v>
       </c>
+      <c r="J12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" s="4">
+        <v>0</v>
+      </c>
       <c r="L12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M12" s="4">
         <v>0</v>
       </c>
-      <c r="N12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="O12" s="4">
-        <v>0</v>
-      </c>
-      <c r="P12" s="2">
+      <c r="N12" s="2">
         <v>29.2</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="5">
+      <c r="B13" s="5">
         <v>44419</v>
       </c>
+      <c r="C13" s="2">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2">
+        <v>7.99</v>
+      </c>
       <c r="E13" s="2">
-        <v>1</v>
+        <v>35080</v>
       </c>
       <c r="F13" s="2">
-        <v>7.99</v>
+        <v>55100</v>
       </c>
       <c r="G13" s="2">
-        <v>35080</v>
+        <v>30500</v>
       </c>
       <c r="H13" s="2">
-        <v>55100</v>
+        <v>1.4</v>
       </c>
       <c r="I13" s="2">
-        <v>30500</v>
-      </c>
-      <c r="J13" s="2">
-        <v>1.4</v>
-      </c>
-      <c r="K13" s="2">
         <v>7.05</v>
       </c>
+      <c r="J13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K13" s="4">
+        <v>0</v>
+      </c>
       <c r="L13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M13" s="4">
         <v>0</v>
       </c>
-      <c r="N13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="O13" s="4">
-        <v>0</v>
-      </c>
-      <c r="P13" s="2">
+      <c r="N13" s="2">
         <v>28.9</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="5">
+      <c r="B14" s="5">
         <v>44419</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="D14" s="2">
+        <v>7.88</v>
+      </c>
+      <c r="E14" s="2">
+        <v>35500</v>
+      </c>
       <c r="F14" s="2">
-        <v>7.88</v>
+        <v>56070</v>
       </c>
       <c r="G14" s="2">
-        <v>35500</v>
+        <v>31590</v>
       </c>
       <c r="H14" s="2">
-        <v>56070</v>
+        <v>0.66</v>
       </c>
       <c r="I14" s="2">
-        <v>31590</v>
-      </c>
-      <c r="J14" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="K14" s="2">
         <v>7.51</v>
       </c>
+      <c r="J14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14" s="4">
+        <v>0</v>
+      </c>
       <c r="L14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M14" s="4">
         <v>0</v>
       </c>
-      <c r="N14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="O14" s="4">
-        <v>0</v>
-      </c>
-      <c r="P14" s="2">
+      <c r="N14" s="2">
         <v>28.7</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="5">
+      <c r="B15" s="5">
         <v>44419</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="D15" s="2">
+        <v>7.84</v>
+      </c>
+      <c r="E15" s="2">
+        <v>35520</v>
+      </c>
       <c r="F15" s="2">
-        <v>7.84</v>
+        <v>53550</v>
       </c>
       <c r="G15" s="2">
-        <v>35520</v>
+        <v>32170</v>
       </c>
       <c r="H15" s="2">
-        <v>53550</v>
+        <v>1.06</v>
       </c>
       <c r="I15" s="2">
-        <v>32170</v>
-      </c>
-      <c r="J15" s="2">
-        <v>1.06</v>
-      </c>
-      <c r="K15" s="2">
         <v>6.01</v>
       </c>
+      <c r="J15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" s="4">
+        <v>0</v>
+      </c>
       <c r="L15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M15" s="4">
         <v>0</v>
       </c>
-      <c r="N15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="O15" s="4">
-        <v>0</v>
-      </c>
-      <c r="P15" s="2">
+      <c r="N15" s="2">
         <v>29.4</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="5">
+      <c r="B16" s="5">
         <v>44419</v>
       </c>
+      <c r="C16" s="2">
+        <v>3</v>
+      </c>
+      <c r="D16" s="2">
+        <v>7.71</v>
+      </c>
       <c r="E16" s="2">
-        <v>3</v>
+        <v>36200</v>
       </c>
       <c r="F16" s="2">
-        <v>7.71</v>
+        <v>54880</v>
       </c>
       <c r="G16" s="2">
-        <v>36200</v>
+        <v>32330</v>
       </c>
       <c r="H16" s="2">
-        <v>54880</v>
+        <v>3.1</v>
       </c>
       <c r="I16" s="2">
-        <v>32330</v>
-      </c>
-      <c r="J16" s="2">
-        <v>3.1</v>
-      </c>
-      <c r="K16" s="2">
         <v>6.2</v>
       </c>
+      <c r="J16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K16" s="4">
+        <v>0</v>
+      </c>
       <c r="L16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M16" s="4">
         <v>0</v>
       </c>
-      <c r="N16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="O16" s="4">
-        <v>0</v>
-      </c>
-      <c r="P16" s="2">
+      <c r="N16" s="2">
         <v>29.7</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="5">
+      <c r="B17" s="5">
         <v>44419</v>
       </c>
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2">
+        <v>7.8</v>
+      </c>
       <c r="E17" s="2">
-        <v>1</v>
+        <v>34810</v>
       </c>
       <c r="F17" s="2">
-        <v>7.8</v>
+        <v>54550</v>
       </c>
       <c r="G17" s="2">
-        <v>34810</v>
+        <v>31570</v>
       </c>
       <c r="H17" s="2">
-        <v>54550</v>
+        <v>1.77</v>
       </c>
       <c r="I17" s="2">
-        <v>31570</v>
-      </c>
-      <c r="J17" s="2">
-        <v>1.77</v>
-      </c>
-      <c r="K17" s="2">
         <v>5.7</v>
       </c>
+      <c r="J17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K17" s="4">
+        <v>0</v>
+      </c>
       <c r="L17" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M17" s="4">
         <v>0</v>
       </c>
-      <c r="N17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="O17" s="4">
-        <v>0</v>
-      </c>
-      <c r="P17" s="2">
+      <c r="N17" s="2">
         <v>28.7</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="5">
+      <c r="B18" s="5">
         <v>44419</v>
       </c>
+      <c r="C18" s="2">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2">
+        <v>7.88</v>
+      </c>
       <c r="E18" s="2">
-        <v>1</v>
+        <v>35880</v>
       </c>
       <c r="F18" s="2">
-        <v>7.88</v>
+        <v>54300</v>
       </c>
       <c r="G18" s="2">
-        <v>35880</v>
+        <v>32080</v>
       </c>
       <c r="H18" s="2">
-        <v>54300</v>
+        <v>0.91</v>
       </c>
       <c r="I18" s="2">
-        <v>32080</v>
-      </c>
-      <c r="J18" s="2">
-        <v>0.91</v>
-      </c>
-      <c r="K18" s="2">
         <v>6.58</v>
       </c>
-      <c r="L18" s="2" t="s">
-        <v>14</v>
+      <c r="J18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K18" s="4">
+        <v>0</v>
+      </c>
+      <c r="L18" s="2">
+        <v>0.04</v>
       </c>
       <c r="M18" s="4">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="N18" s="2">
-        <v>0.04</v>
-      </c>
-      <c r="O18" s="4">
-        <v>0.04</v>
-      </c>
-      <c r="P18" s="2">
         <v>28.6</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="5">
+      <c r="B19" s="5">
         <v>44419</v>
       </c>
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2">
+        <v>7.48</v>
+      </c>
       <c r="E19" s="2">
-        <v>1</v>
+        <v>36160</v>
       </c>
       <c r="F19" s="2">
-        <v>6.2</v>
+        <v>54370</v>
       </c>
       <c r="G19" s="2">
-        <v>36160</v>
+        <v>32130</v>
       </c>
       <c r="H19" s="2">
-        <v>54370</v>
+        <v>1.71</v>
       </c>
       <c r="I19" s="2">
-        <v>32130</v>
-      </c>
-      <c r="J19" s="2">
-        <v>1.71</v>
-      </c>
-      <c r="K19" s="2">
         <v>6.43</v>
       </c>
+      <c r="J19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K19" s="4">
+        <v>0</v>
+      </c>
       <c r="L19" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M19" s="4">
         <v>0</v>
       </c>
-      <c r="N19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="O19" s="4">
-        <v>0</v>
-      </c>
-      <c r="P19" s="2">
+      <c r="N19" s="2">
         <v>28.7</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="5">
+      <c r="B20" s="5">
         <v>44419</v>
       </c>
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2">
+        <v>7.68</v>
+      </c>
       <c r="E20" s="2">
-        <v>1</v>
+        <v>36640</v>
       </c>
       <c r="F20" s="2">
-        <v>7.68</v>
+        <v>53620</v>
       </c>
       <c r="G20" s="2">
-        <v>36640</v>
+        <v>31090</v>
       </c>
       <c r="H20" s="2">
-        <v>53620</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="I20" s="2">
-        <v>31090</v>
-      </c>
-      <c r="J20" s="2">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="K20" s="2">
         <v>5.56</v>
       </c>
+      <c r="J20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K20" s="4">
+        <v>0</v>
+      </c>
       <c r="L20" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M20" s="4">
         <v>0</v>
       </c>
-      <c r="N20" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="O20" s="4">
-        <v>0</v>
-      </c>
-      <c r="P20" s="2">
+      <c r="N20" s="2">
         <v>28.8</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="5">
+      <c r="B21" s="5">
         <v>44419</v>
       </c>
+      <c r="C21" s="2">
+        <v>10</v>
+      </c>
+      <c r="D21" s="2">
+        <v>7.25</v>
+      </c>
       <c r="E21" s="2">
-        <v>10</v>
+        <v>36030</v>
       </c>
       <c r="F21" s="2">
-        <v>7.25</v>
+        <v>53210</v>
       </c>
       <c r="G21" s="2">
-        <v>36030</v>
+        <v>32070</v>
       </c>
       <c r="H21" s="2">
-        <v>53210</v>
+        <v>26.2</v>
       </c>
       <c r="I21" s="2">
-        <v>32070</v>
-      </c>
-      <c r="J21" s="2">
-        <v>26.2</v>
-      </c>
-      <c r="K21" s="2">
         <v>0.26</v>
       </c>
+      <c r="J21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K21" s="4">
+        <v>0</v>
+      </c>
       <c r="L21" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M21" s="4">
         <v>0</v>
       </c>
-      <c r="N21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="O21" s="4">
-        <v>0</v>
-      </c>
-      <c r="P21" s="2">
+      <c r="N21" s="2">
         <v>28.6</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="5">
+      <c r="B22" s="5">
         <v>44419</v>
       </c>
+      <c r="C22" s="2">
+        <v>2</v>
+      </c>
+      <c r="D22" s="2">
+        <v>7.65</v>
+      </c>
       <c r="E22" s="2">
-        <v>2</v>
+        <v>30840</v>
       </c>
       <c r="F22" s="2">
-        <v>7.65</v>
+        <v>54920</v>
       </c>
       <c r="G22" s="2">
-        <v>30840</v>
+        <v>31850</v>
       </c>
       <c r="H22" s="2">
-        <v>54920</v>
+        <v>2.98</v>
       </c>
       <c r="I22" s="2">
-        <v>31850</v>
-      </c>
-      <c r="J22" s="2">
-        <v>2.98</v>
-      </c>
-      <c r="K22" s="2">
         <v>5.48</v>
       </c>
+      <c r="J22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K22" s="4">
+        <v>0</v>
+      </c>
       <c r="L22" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M22" s="4">
         <v>0</v>
       </c>
-      <c r="N22" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="O22" s="4">
-        <v>0</v>
-      </c>
-      <c r="P22" s="2">
+      <c r="N22" s="2">
         <v>29.2</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="5">
+      <c r="B23" s="5">
         <v>44419</v>
       </c>
+      <c r="C23" s="2">
+        <v>1</v>
+      </c>
+      <c r="D23" s="2">
+        <v>7.71</v>
+      </c>
       <c r="E23" s="2">
-        <v>1</v>
+        <v>36730</v>
       </c>
       <c r="F23" s="2">
-        <v>7.71</v>
+        <v>54830</v>
       </c>
       <c r="G23" s="2">
-        <v>36730</v>
+        <v>31440</v>
       </c>
       <c r="H23" s="2">
-        <v>54830</v>
+        <v>1.02</v>
       </c>
       <c r="I23" s="2">
-        <v>31440</v>
-      </c>
-      <c r="J23" s="2">
-        <v>1.02</v>
-      </c>
-      <c r="K23" s="2">
         <v>6.12</v>
       </c>
+      <c r="J23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K23" s="4">
+        <v>0</v>
+      </c>
       <c r="L23" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M23" s="4">
         <v>0</v>
       </c>
-      <c r="N23" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="O23" s="4">
-        <v>0</v>
-      </c>
-      <c r="P23" s="2">
+      <c r="N23" s="2">
         <v>28.8</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="5">
+      <c r="B24" s="5">
         <v>44419</v>
       </c>
+      <c r="C24" s="2">
+        <v>1</v>
+      </c>
+      <c r="D24" s="2">
+        <v>7.91</v>
+      </c>
       <c r="E24" s="2">
-        <v>1</v>
+        <v>36010</v>
       </c>
       <c r="F24" s="2">
-        <v>7.91</v>
+        <v>53900</v>
       </c>
       <c r="G24" s="2">
-        <v>36010</v>
+        <v>29750</v>
       </c>
       <c r="H24" s="2">
-        <v>53900</v>
+        <v>1.07</v>
       </c>
       <c r="I24" s="2">
-        <v>29750</v>
-      </c>
-      <c r="J24" s="2">
-        <v>1.07</v>
-      </c>
-      <c r="K24" s="2">
         <v>6.72</v>
       </c>
+      <c r="J24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K24" s="4">
+        <v>0</v>
+      </c>
       <c r="L24" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M24" s="4">
         <v>0</v>
       </c>
-      <c r="N24" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="O24" s="4">
-        <v>0</v>
-      </c>
-      <c r="P24" s="2">
+      <c r="N24" s="2">
         <v>28.6</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="5">
+      <c r="B25" s="5">
         <v>44419</v>
       </c>
+      <c r="C25" s="2">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2">
+        <v>7.53</v>
+      </c>
       <c r="E25" s="2">
-        <v>1</v>
+        <v>34580</v>
       </c>
       <c r="F25" s="2">
-        <v>7.53</v>
+        <v>54380</v>
       </c>
       <c r="G25" s="2">
-        <v>34580</v>
+        <v>31160</v>
       </c>
       <c r="H25" s="2">
-        <v>54380</v>
+        <v>2.14</v>
       </c>
       <c r="I25" s="2">
-        <v>31160</v>
-      </c>
-      <c r="J25" s="2">
-        <v>2.14</v>
-      </c>
-      <c r="K25" s="2">
         <v>5.78</v>
       </c>
+      <c r="J25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K25" s="4">
+        <v>0</v>
+      </c>
       <c r="L25" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M25" s="4">
         <v>0</v>
       </c>
-      <c r="N25" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="O25" s="4">
-        <v>0</v>
-      </c>
-      <c r="P25" s="2">
+      <c r="N25" s="2">
         <v>28.8</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="5">
+      <c r="B26" s="5">
         <v>44419</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="D26" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="E26" s="2">
+        <v>34580</v>
+      </c>
       <c r="F26" s="2">
-        <v>7.5</v>
+        <v>53920</v>
       </c>
       <c r="G26" s="2">
-        <v>34580</v>
+        <v>31060</v>
       </c>
       <c r="H26" s="2">
-        <v>53920</v>
+        <v>0.6</v>
       </c>
       <c r="I26" s="2">
-        <v>31060</v>
-      </c>
-      <c r="J26" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="K26" s="2">
         <v>7.21</v>
       </c>
+      <c r="J26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K26" s="4">
+        <v>0</v>
+      </c>
       <c r="L26" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M26" s="4">
         <v>0</v>
       </c>
-      <c r="N26" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="O26" s="4">
-        <v>0</v>
-      </c>
-      <c r="P26" s="2">
+      <c r="N26" s="2">
         <v>29.2</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="5">
+      <c r="B27" s="5">
         <v>44419</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="D27" s="2">
+        <v>7.92</v>
+      </c>
+      <c r="E27" s="2">
+        <v>36590</v>
+      </c>
       <c r="F27" s="2">
-        <v>7.92</v>
+        <v>54840</v>
       </c>
       <c r="G27" s="2">
-        <v>36590</v>
+        <v>32230</v>
       </c>
       <c r="H27" s="2">
-        <v>54840</v>
+        <v>0.53</v>
       </c>
       <c r="I27" s="2">
-        <v>32230</v>
+        <v>6.51</v>
       </c>
       <c r="J27" s="2">
-        <v>0.53</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="K27" s="2">
-        <v>6.51</v>
-      </c>
-      <c r="L27" s="2">
         <v>0.14000000000000001</v>
       </c>
+      <c r="L27" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="M27" s="2">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="N27" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="O27" s="2">
-        <v>0</v>
-      </c>
-      <c r="P27" s="2">
+        <v>0</v>
+      </c>
+      <c r="N27" s="2">
         <v>28.8</v>
       </c>
     </row>
@@ -1871,7 +1794,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2004,6 +1927,9 @@
       <c r="B12" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="C12" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
@@ -2012,6 +1938,9 @@
       <c r="B13" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="C13" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
@@ -2020,6 +1949,9 @@
       <c r="B14" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="C14" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
@@ -2028,6 +1960,9 @@
       <c r="B15" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="C15" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
@@ -2036,29 +1971,41 @@
       <c r="B16" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>48</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>